<commit_message>
images go now to img directory, update that in readme
</commit_message>
<xml_diff>
--- a/2019_nCoV.xlsx
+++ b/2019_nCoV.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5448" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5640" uniqueCount="411">
   <si>
     <t>Province/State</t>
   </si>
@@ -1224,6 +1224,30 @@
   <si>
     <t>2/5/20 21:53</t>
   </si>
+  <si>
+    <t>2/6/20 23:23</t>
+  </si>
+  <si>
+    <t>2/6/20 23:33</t>
+  </si>
+  <si>
+    <t>2/7/20 0:53</t>
+  </si>
+  <si>
+    <t>2/7/20 0:03</t>
+  </si>
+  <si>
+    <t>2/7/20 0:33</t>
+  </si>
+  <si>
+    <t>2/7/20 0:43</t>
+  </si>
+  <si>
+    <t>2/6/20 23:03</t>
+  </si>
+  <si>
+    <t>2/6/20 23:43</t>
+  </si>
 </sst>
 </file>
 
@@ -1580,7 +1604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1976"/>
+  <dimension ref="A1:F2047"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -39657,6 +39681,1363 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1977" spans="1:6">
+      <c r="A1977" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1977" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1977" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1977">
+        <v>22112</v>
+      </c>
+      <c r="E1977">
+        <v>817</v>
+      </c>
+      <c r="F1977">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="1978" spans="1:6">
+      <c r="A1978" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1978" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1978" t="s">
+        <v>372</v>
+      </c>
+      <c r="D1978">
+        <v>970</v>
+      </c>
+      <c r="E1978">
+        <v>69</v>
+      </c>
+      <c r="F1978">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1979" spans="1:6">
+      <c r="A1979" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1979" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1979" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1979">
+        <v>954</v>
+      </c>
+      <c r="E1979">
+        <v>94</v>
+      </c>
+      <c r="F1979">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1980" spans="1:6">
+      <c r="A1980" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1980" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1980" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1980">
+        <v>851</v>
+      </c>
+      <c r="E1980">
+        <v>56</v>
+      </c>
+      <c r="F1980">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1981" spans="1:6">
+      <c r="A1981" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1981" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1981" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1981">
+        <v>711</v>
+      </c>
+      <c r="E1981">
+        <v>81</v>
+      </c>
+      <c r="F1981">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1982" spans="1:6">
+      <c r="A1982" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1982" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1982" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1982">
+        <v>600</v>
+      </c>
+      <c r="E1982">
+        <v>37</v>
+      </c>
+      <c r="F1982">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1983" spans="1:6">
+      <c r="A1983" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1983" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1983" t="s">
+        <v>377</v>
+      </c>
+      <c r="D1983">
+        <v>591</v>
+      </c>
+      <c r="E1983">
+        <v>34</v>
+      </c>
+      <c r="F1983">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1984" spans="1:6">
+      <c r="A1984" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1984" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1984" t="s">
+        <v>404</v>
+      </c>
+      <c r="D1984">
+        <v>411</v>
+      </c>
+      <c r="E1984">
+        <v>24</v>
+      </c>
+      <c r="F1984">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1985" spans="1:6">
+      <c r="A1985" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1985" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1985" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1985">
+        <v>373</v>
+      </c>
+      <c r="E1985">
+        <v>34</v>
+      </c>
+      <c r="F1985">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1986" spans="1:6">
+      <c r="A1986" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1986" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1986" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1986">
+        <v>347</v>
+      </c>
+      <c r="E1986">
+        <v>27</v>
+      </c>
+      <c r="F1986">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1987" spans="1:6">
+      <c r="A1987" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1987" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1987" t="s">
+        <v>405</v>
+      </c>
+      <c r="D1987">
+        <v>344</v>
+      </c>
+      <c r="E1987">
+        <v>37</v>
+      </c>
+      <c r="F1987">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1988" spans="1:6">
+      <c r="A1988" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1988" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1988" t="s">
+        <v>381</v>
+      </c>
+      <c r="D1988">
+        <v>274</v>
+      </c>
+      <c r="E1988">
+        <v>31</v>
+      </c>
+      <c r="F1988">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1989" spans="1:6">
+      <c r="A1989" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1989" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1989" t="s">
+        <v>406</v>
+      </c>
+      <c r="D1989">
+        <v>269</v>
+      </c>
+      <c r="E1989">
+        <v>25</v>
+      </c>
+      <c r="F1989">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:6">
+      <c r="A1990" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1990" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1990" t="s">
+        <v>383</v>
+      </c>
+      <c r="D1990">
+        <v>227</v>
+      </c>
+      <c r="E1990">
+        <v>8</v>
+      </c>
+      <c r="F1990">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:6">
+      <c r="A1991" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1991" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1991" t="s">
+        <v>384</v>
+      </c>
+      <c r="D1991">
+        <v>215</v>
+      </c>
+      <c r="E1991">
+        <v>14</v>
+      </c>
+      <c r="F1991">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1992" spans="1:6">
+      <c r="A1992" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1992" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1992" t="s">
+        <v>385</v>
+      </c>
+      <c r="D1992">
+        <v>173</v>
+      </c>
+      <c r="E1992">
+        <v>9</v>
+      </c>
+      <c r="F1992">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:6">
+      <c r="A1993" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1993" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1993" t="s">
+        <v>407</v>
+      </c>
+      <c r="D1993">
+        <v>172</v>
+      </c>
+      <c r="E1993">
+        <v>17</v>
+      </c>
+      <c r="F1993">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:6">
+      <c r="A1994" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1994" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1994" t="s">
+        <v>408</v>
+      </c>
+      <c r="D1994">
+        <v>171</v>
+      </c>
+      <c r="E1994">
+        <v>16</v>
+      </c>
+      <c r="F1994">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:6">
+      <c r="A1995" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1995" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1995" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1995">
+        <v>133</v>
+      </c>
+      <c r="E1995">
+        <v>7</v>
+      </c>
+      <c r="F1995">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:6">
+      <c r="A1996" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1996" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1996" t="s">
+        <v>406</v>
+      </c>
+      <c r="D1996">
+        <v>106</v>
+      </c>
+      <c r="E1996">
+        <v>8</v>
+      </c>
+      <c r="F1996">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:6">
+      <c r="A1997" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1997" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1997" t="s">
+        <v>409</v>
+      </c>
+      <c r="D1997">
+        <v>96</v>
+      </c>
+      <c r="E1997">
+        <v>12</v>
+      </c>
+      <c r="F1997">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:6">
+      <c r="A1998" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1998" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1998" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1998">
+        <v>94</v>
+      </c>
+      <c r="E1998">
+        <v>5</v>
+      </c>
+      <c r="F1998">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:6">
+      <c r="A1999" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1999" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1999" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1999">
+        <v>79</v>
+      </c>
+      <c r="E1999">
+        <v>2</v>
+      </c>
+      <c r="F1999">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:6">
+      <c r="A2000" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2000" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2000" t="s">
+        <v>392</v>
+      </c>
+      <c r="D2000">
+        <v>71</v>
+      </c>
+      <c r="E2000">
+        <v>6</v>
+      </c>
+      <c r="F2000">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2001" spans="1:6">
+      <c r="A2001" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2001" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2001" t="s">
+        <v>408</v>
+      </c>
+      <c r="D2001">
+        <v>65</v>
+      </c>
+      <c r="E2001">
+        <v>4</v>
+      </c>
+      <c r="F2001">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:6">
+      <c r="A2002" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2002" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2002" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2002">
+        <v>62</v>
+      </c>
+      <c r="E2002">
+        <v>6</v>
+      </c>
+      <c r="F2002">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:6">
+      <c r="A2003" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2003" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2003" t="s">
+        <v>394</v>
+      </c>
+      <c r="D2003">
+        <v>46</v>
+      </c>
+      <c r="E2003">
+        <v>4</v>
+      </c>
+      <c r="F2003">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:6">
+      <c r="B2004" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2004" t="s">
+        <v>395</v>
+      </c>
+      <c r="D2004">
+        <v>45</v>
+      </c>
+      <c r="E2004">
+        <v>1</v>
+      </c>
+      <c r="F2004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2005" spans="1:6">
+      <c r="A2005" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2005" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2005" t="s">
+        <v>396</v>
+      </c>
+      <c r="D2005">
+        <v>40</v>
+      </c>
+      <c r="E2005">
+        <v>1</v>
+      </c>
+      <c r="F2005">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2006" spans="1:6">
+      <c r="A2006" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2006" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2006" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2006">
+        <v>36</v>
+      </c>
+      <c r="E2006">
+        <v>0</v>
+      </c>
+      <c r="F2006">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2007" spans="1:6">
+      <c r="B2007" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2007" t="s">
+        <v>366</v>
+      </c>
+      <c r="D2007">
+        <v>28</v>
+      </c>
+      <c r="E2007">
+        <v>0</v>
+      </c>
+      <c r="F2007">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2008" spans="1:6">
+      <c r="B2008" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2008" t="s">
+        <v>325</v>
+      </c>
+      <c r="D2008">
+        <v>25</v>
+      </c>
+      <c r="E2008">
+        <v>5</v>
+      </c>
+      <c r="F2008">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2009" spans="1:6">
+      <c r="A2009" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2009" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2009" t="s">
+        <v>398</v>
+      </c>
+      <c r="D2009">
+        <v>24</v>
+      </c>
+      <c r="E2009">
+        <v>0</v>
+      </c>
+      <c r="F2009">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2010" spans="1:6">
+      <c r="B2010" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2010" t="s">
+        <v>395</v>
+      </c>
+      <c r="D2010">
+        <v>23</v>
+      </c>
+      <c r="E2010">
+        <v>0</v>
+      </c>
+      <c r="F2010">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2011" spans="1:6">
+      <c r="A2011" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2011" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2011" t="s">
+        <v>396</v>
+      </c>
+      <c r="D2011">
+        <v>18</v>
+      </c>
+      <c r="E2011">
+        <v>3</v>
+      </c>
+      <c r="F2011">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:6">
+      <c r="A2012" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2012" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2012" t="s">
+        <v>399</v>
+      </c>
+      <c r="D2012">
+        <v>16</v>
+      </c>
+      <c r="E2012">
+        <v>1</v>
+      </c>
+      <c r="F2012">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2013" spans="1:6">
+      <c r="B2013" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2013" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2013">
+        <v>12</v>
+      </c>
+      <c r="E2013">
+        <v>0</v>
+      </c>
+      <c r="F2013">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2014" spans="1:6">
+      <c r="B2014" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2014" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2014">
+        <v>12</v>
+      </c>
+      <c r="E2014">
+        <v>0</v>
+      </c>
+      <c r="F2014">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2015" spans="1:6">
+      <c r="A2015" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2015" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2015" t="s">
+        <v>393</v>
+      </c>
+      <c r="D2015">
+        <v>10</v>
+      </c>
+      <c r="E2015">
+        <v>1</v>
+      </c>
+      <c r="F2015">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2016" spans="1:6">
+      <c r="B2016" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2016" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2016">
+        <v>10</v>
+      </c>
+      <c r="E2016">
+        <v>1</v>
+      </c>
+      <c r="F2016">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2017" spans="1:6">
+      <c r="B2017" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2017" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2017">
+        <v>6</v>
+      </c>
+      <c r="E2017">
+        <v>0</v>
+      </c>
+      <c r="F2017">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2018" spans="1:6">
+      <c r="B2018" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2018" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2018">
+        <v>5</v>
+      </c>
+      <c r="E2018">
+        <v>0</v>
+      </c>
+      <c r="F2018">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2019" spans="1:6">
+      <c r="A2019" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2019" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2019" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2019">
+        <v>4</v>
+      </c>
+      <c r="E2019">
+        <v>2</v>
+      </c>
+      <c r="F2019">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2020" spans="1:6">
+      <c r="A2020" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2020" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2020" t="s">
+        <v>395</v>
+      </c>
+      <c r="D2020">
+        <v>4</v>
+      </c>
+      <c r="E2020">
+        <v>0</v>
+      </c>
+      <c r="F2020">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2021" spans="1:6">
+      <c r="A2021" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2021" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2021" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2021">
+        <v>4</v>
+      </c>
+      <c r="E2021">
+        <v>0</v>
+      </c>
+      <c r="F2021">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2022" spans="1:6">
+      <c r="B2022" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2022" t="s">
+        <v>285</v>
+      </c>
+      <c r="D2022">
+        <v>3</v>
+      </c>
+      <c r="E2022">
+        <v>0</v>
+      </c>
+      <c r="F2022">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2023" spans="1:6">
+      <c r="A2023" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2023" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2023" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2023">
+        <v>2</v>
+      </c>
+      <c r="E2023">
+        <v>0</v>
+      </c>
+      <c r="F2023">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2024" spans="1:6">
+      <c r="A2024" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2024" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2024" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2024">
+        <v>2</v>
+      </c>
+      <c r="E2024">
+        <v>0</v>
+      </c>
+      <c r="F2024">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2025" spans="1:6">
+      <c r="A2025" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2025" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2025" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2025">
+        <v>2</v>
+      </c>
+      <c r="E2025">
+        <v>0</v>
+      </c>
+      <c r="F2025">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2026" spans="1:6">
+      <c r="B2026" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2026" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2026">
+        <v>2</v>
+      </c>
+      <c r="E2026">
+        <v>0</v>
+      </c>
+      <c r="F2026">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2027" spans="1:6">
+      <c r="B2027" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2027" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2027">
+        <v>2</v>
+      </c>
+      <c r="E2027">
+        <v>0</v>
+      </c>
+      <c r="F2027">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2028" spans="1:6">
+      <c r="B2028" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2028" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2028">
+        <v>2</v>
+      </c>
+      <c r="E2028">
+        <v>0</v>
+      </c>
+      <c r="F2028">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2029" spans="1:6">
+      <c r="B2029" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2029" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2029">
+        <v>2</v>
+      </c>
+      <c r="E2029">
+        <v>0</v>
+      </c>
+      <c r="F2029">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2030" spans="1:6">
+      <c r="A2030" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2030" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2030" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2030">
+        <v>2</v>
+      </c>
+      <c r="E2030">
+        <v>0</v>
+      </c>
+      <c r="F2030">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2031" spans="1:6">
+      <c r="A2031" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2031" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2031" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2031">
+        <v>2</v>
+      </c>
+      <c r="E2031">
+        <v>0</v>
+      </c>
+      <c r="F2031">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2032" spans="1:6">
+      <c r="A2032" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2032" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2032" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2032">
+        <v>2</v>
+      </c>
+      <c r="E2032">
+        <v>0</v>
+      </c>
+      <c r="F2032">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2033" spans="1:6">
+      <c r="B2033" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2033" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2033">
+        <v>1</v>
+      </c>
+      <c r="E2033">
+        <v>0</v>
+      </c>
+      <c r="F2033">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2034" spans="1:6">
+      <c r="B2034" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2034" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2034">
+        <v>1</v>
+      </c>
+      <c r="E2034">
+        <v>0</v>
+      </c>
+      <c r="F2034">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2035" spans="1:6">
+      <c r="A2035" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2035" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2035" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2035">
+        <v>1</v>
+      </c>
+      <c r="E2035">
+        <v>0</v>
+      </c>
+      <c r="F2035">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2036" spans="1:6">
+      <c r="B2036" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2036" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2036">
+        <v>1</v>
+      </c>
+      <c r="E2036">
+        <v>0</v>
+      </c>
+      <c r="F2036">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2037" spans="1:6">
+      <c r="A2037" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2037" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2037" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2037">
+        <v>1</v>
+      </c>
+      <c r="E2037">
+        <v>0</v>
+      </c>
+      <c r="F2037">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2038" spans="1:6">
+      <c r="B2038" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2038" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2038">
+        <v>1</v>
+      </c>
+      <c r="E2038">
+        <v>0</v>
+      </c>
+      <c r="F2038">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2039" spans="1:6">
+      <c r="B2039" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2039" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2039">
+        <v>1</v>
+      </c>
+      <c r="E2039">
+        <v>0</v>
+      </c>
+      <c r="F2039">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2040" spans="1:6">
+      <c r="B2040" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2040" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2040">
+        <v>1</v>
+      </c>
+      <c r="E2040">
+        <v>0</v>
+      </c>
+      <c r="F2040">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2041" spans="1:6">
+      <c r="B2041" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2041" t="s">
+        <v>297</v>
+      </c>
+      <c r="D2041">
+        <v>1</v>
+      </c>
+      <c r="E2041">
+        <v>0</v>
+      </c>
+      <c r="F2041">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2042" spans="1:6">
+      <c r="A2042" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2042" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2042" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2042">
+        <v>1</v>
+      </c>
+      <c r="E2042">
+        <v>0</v>
+      </c>
+      <c r="F2042">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2043" spans="1:6">
+      <c r="A2043" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2043" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2043" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2043">
+        <v>1</v>
+      </c>
+      <c r="E2043">
+        <v>0</v>
+      </c>
+      <c r="F2043">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2044" spans="1:6">
+      <c r="A2044" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2044" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2044" t="s">
+        <v>402</v>
+      </c>
+      <c r="D2044">
+        <v>1</v>
+      </c>
+      <c r="E2044">
+        <v>0</v>
+      </c>
+      <c r="F2044">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2045" spans="1:6">
+      <c r="A2045" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2045" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2045" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2045">
+        <v>1</v>
+      </c>
+      <c r="E2045">
+        <v>0</v>
+      </c>
+      <c r="F2045">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2046" spans="1:6">
+      <c r="A2046" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2046" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2046" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2046">
+        <v>1</v>
+      </c>
+      <c r="E2046">
+        <v>0</v>
+      </c>
+      <c r="F2046">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2047" spans="1:6">
+      <c r="A2047" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2047" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2047" t="s">
+        <v>292</v>
+      </c>
+      <c r="D2047">
+        <v>1</v>
+      </c>
+      <c r="E2047">
+        <v>0</v>
+      </c>
+      <c r="F2047">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>